<commit_message>
--weekly-report worksgit add .git add .git add .
</commit_message>
<xml_diff>
--- a/revamp/weekly_report.xlsx
+++ b/revamp/weekly_report.xlsx
@@ -479,7 +479,7 @@
         <v>1.12</v>
       </c>
       <c r="D3">
-        <v>845.0190145631053</v>
+        <v>843.6235380817586</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -493,7 +493,7 @@
         <v>-45.4</v>
       </c>
       <c r="D4">
-        <v>555.6083742765481</v>
+        <v>147.1422559759127</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -507,7 +507,7 @@
         <v>-24.32</v>
       </c>
       <c r="D5">
-        <v>157.6837929772965</v>
+        <v>157.4233917072693</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -521,7 +521,7 @@
         <v>85.65000000000001</v>
       </c>
       <c r="D6">
-        <v>2120.00862222459</v>
+        <v>707.2250046894603</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -535,7 +535,7 @@
         <v>-28.54</v>
       </c>
       <c r="D7">
-        <v>405.1225666606358</v>
+        <v>404.4535414622738</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -549,7 +549,7 @@
         <v>-36.57</v>
       </c>
       <c r="D8">
-        <v>237.5869551366882</v>
+        <v>237.1946006423465</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -591,7 +591,7 @@
         <v>-7.83</v>
       </c>
       <c r="D11">
-        <v>434.3621302284947</v>
+        <v>434.393405838844</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -605,7 +605,7 @@
         <v>45.15</v>
       </c>
       <c r="D12">
-        <v>2048.23054487138</v>
+        <v>827.426200917405</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -619,7 +619,7 @@
         <v>-23.4</v>
       </c>
       <c r="D13">
-        <v>838.3455422848089</v>
+        <v>836.9610864709889</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -633,7 +633,7 @@
         <v>28.85</v>
       </c>
       <c r="D14">
-        <v>721.1911787192519</v>
+        <v>720.0001932963053</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -647,7 +647,7 @@
         <v>-25.5</v>
       </c>
       <c r="D15">
-        <v>437.670269290659</v>
+        <v>436.9474943508601</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -661,7 +661,7 @@
         <v>30.52</v>
       </c>
       <c r="D16">
-        <v>542.4897312151949</v>
+        <v>542.5287923954203</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -675,7 +675,7 @@
         <v>-76.03</v>
       </c>
       <c r="D17">
-        <v>68.47266731258281</v>
+        <v>68.35959057087283</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -685,8 +685,11 @@
       <c r="B18">
         <v>5.6</v>
       </c>
+      <c r="C18">
+        <v>-19.89</v>
+      </c>
       <c r="D18">
-        <v>11058.8688500774</v>
+        <v>8010.756556715879</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test if data commited
</commit_message>
<xml_diff>
--- a/revamp/weekly_report.xlsx
+++ b/revamp/weekly_report.xlsx
@@ -459,13 +459,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>3.89</v>
+        <v>-1.08</v>
       </c>
       <c r="C2">
-        <v>-35.02</v>
+        <v>-36.61</v>
       </c>
       <c r="D2">
-        <v>682.1279213483147</v>
+        <v>665.4580300886175</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -473,13 +473,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>7.8</v>
+        <v>2.58</v>
       </c>
       <c r="C3">
-        <v>1.12</v>
+        <v>2.57</v>
       </c>
       <c r="D3">
-        <v>843.6235380817586</v>
+        <v>852.2645515146485</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -487,13 +487,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>8.039999999999999</v>
+        <v>1.59</v>
       </c>
       <c r="C4">
-        <v>-45.4</v>
+        <v>-44.76</v>
       </c>
       <c r="D4">
-        <v>147.1422559759127</v>
+        <v>148.2422796806763</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -501,13 +501,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>9.43</v>
+        <v>4.5</v>
       </c>
       <c r="C5">
-        <v>-24.32</v>
+        <v>-23.07</v>
       </c>
       <c r="D5">
-        <v>157.4233917072693</v>
+        <v>159.3633706374936</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -515,13 +515,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>3.55</v>
+        <v>2.01</v>
       </c>
       <c r="C6">
-        <v>85.65000000000001</v>
+        <v>87.84999999999999</v>
       </c>
       <c r="D6">
-        <v>707.2250046894603</v>
+        <v>712.7101401789072</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -529,13 +529,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>6.66</v>
+        <v>1.21</v>
       </c>
       <c r="C7">
-        <v>-28.54</v>
+        <v>-27.84</v>
       </c>
       <c r="D7">
-        <v>404.4535414622738</v>
+        <v>406.7558751760207</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -543,13 +543,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>7.9</v>
+        <v>-2.73</v>
       </c>
       <c r="C8">
-        <v>-36.57</v>
+        <v>-37.17</v>
       </c>
       <c r="D8">
-        <v>237.1946006423465</v>
+        <v>233.984900923297</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -557,13 +557,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>10.56</v>
+        <v>-4.5</v>
       </c>
       <c r="C9">
-        <v>-72.93000000000001</v>
+        <v>-74.67</v>
       </c>
       <c r="D9">
-        <v>331.9495389678472</v>
+        <v>310.5968891251165</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -571,13 +571,13 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>0.48</v>
+        <v>1.7</v>
       </c>
       <c r="C10">
-        <v>4.66</v>
+        <v>6.65</v>
       </c>
       <c r="D10">
-        <v>633</v>
+        <v>645</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -585,13 +585,13 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>5.13</v>
+        <v>0.67</v>
       </c>
       <c r="C11">
-        <v>-7.83</v>
+        <v>-7.25</v>
       </c>
       <c r="D11">
-        <v>434.393405838844</v>
+        <v>434.3055113215779</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -599,13 +599,13 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>14.59</v>
+        <v>-1.69</v>
       </c>
       <c r="C12">
-        <v>45.15</v>
+        <v>44.31</v>
       </c>
       <c r="D12">
-        <v>827.426200917405</v>
+        <v>817.257859779848</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -613,13 +613,13 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>5.36</v>
+        <v>5.72</v>
       </c>
       <c r="C13">
-        <v>-23.4</v>
+        <v>-19.32</v>
       </c>
       <c r="D13">
-        <v>836.9610864709889</v>
+        <v>877.9071361015275</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -627,13 +627,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>4.04</v>
+        <v>0.82</v>
       </c>
       <c r="C14">
-        <v>28.85</v>
+        <v>29.07</v>
       </c>
       <c r="D14">
-        <v>720.0001932963053</v>
+        <v>718.3415849059797</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -641,13 +641,13 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>1.49</v>
+        <v>0.43</v>
       </c>
       <c r="C15">
-        <v>-25.5</v>
+        <v>-24.5</v>
       </c>
       <c r="D15">
-        <v>436.9474943508601</v>
+        <v>441.0003016115479</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -655,13 +655,13 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>-0.37</v>
+        <v>3.25</v>
       </c>
       <c r="C16">
-        <v>30.52</v>
+        <v>32.91</v>
       </c>
       <c r="D16">
-        <v>542.5287923954203</v>
+        <v>548.8453146526005</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -669,13 +669,13 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>12.99</v>
+        <v>4.83</v>
       </c>
       <c r="C17">
-        <v>-76.03</v>
+        <v>-75.68000000000001</v>
       </c>
       <c r="D17">
-        <v>68.35959057087283</v>
+        <v>69.05455730801823</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -683,13 +683,13 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>5.6</v>
+        <v>1.31</v>
       </c>
       <c r="C18">
-        <v>-19.89</v>
+        <v>-19.59</v>
       </c>
       <c r="D18">
-        <v>8010.756556715879</v>
+        <v>8041.088303005878</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cash position working. Starting on populating spreadsheet
</commit_message>
<xml_diff>
--- a/revamp/weekly_report.xlsx
+++ b/revamp/weekly_report.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Weekly_Update" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Company Name</t>
   </si>
@@ -77,12 +77,21 @@
   </si>
   <si>
     <t>Total Portfolio</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>---</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -135,8 +144,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -434,23 +446,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="4" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -458,13 +473,13 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>-7.86</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>-34.34</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>681.9170118713379</v>
       </c>
     </row>
@@ -472,13 +487,13 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>2.14</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>12.79</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>1261.177746458024</v>
       </c>
     </row>
@@ -486,13 +501,13 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>2.15</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>-38.4</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>252.3617378620049</v>
       </c>
     </row>
@@ -500,13 +515,13 @@
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>-0.64</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>-17.96</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>210.7299412096491</v>
       </c>
     </row>
@@ -514,13 +529,13 @@
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>8.289999999999999</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>128.21</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>1286.713603658671</v>
       </c>
     </row>
@@ -528,13 +543,13 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>-0.61</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>-31.42</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>498.7693075478464</v>
       </c>
     </row>
@@ -542,13 +557,13 @@
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>-1.81</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>-30.93</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>318.9457993599315</v>
       </c>
     </row>
@@ -556,13 +571,13 @@
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>-1.26</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>-68.77</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>376.9500045776367</v>
       </c>
     </row>
@@ -570,13 +585,13 @@
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>0.2</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>-2.83</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>587.6999999999999</v>
       </c>
     </row>
@@ -584,13 +599,13 @@
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>1.85</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>6.61</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>544.8237330000001</v>
       </c>
     </row>
@@ -598,13 +613,13 @@
       <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>-5.65</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>46.12</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>872.879927029953</v>
       </c>
     </row>
@@ -612,13 +627,13 @@
       <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>7.78</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>-12.26</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>1308.006625290777</v>
       </c>
     </row>
@@ -626,13 +641,13 @@
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>-1.68</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>37.09</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>240.6900110959508</v>
       </c>
     </row>
@@ -640,13 +655,13 @@
       <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>-2.61</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>-28.54</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>497.9412672558684</v>
       </c>
     </row>
@@ -654,13 +669,13 @@
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>-1.01</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>26.58</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>567.4945843380776</v>
       </c>
     </row>
@@ -668,13 +683,13 @@
       <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>-0.72</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>-72.61</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>104.856307376423</v>
       </c>
     </row>
@@ -682,14 +697,28 @@
       <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>1.15</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>-3.88</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>9611.957607932152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1229.532809899639</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1335.176621862619</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
historical values and dividends
</commit_message>
<xml_diff>
--- a/revamp/weekly_report.xlsx
+++ b/revamp/weekly_report.xlsx
@@ -474,13 +474,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>-7.86</v>
+        <v>-10.05</v>
       </c>
       <c r="C2" s="1">
-        <v>-34.34</v>
+        <v>-36.67</v>
       </c>
       <c r="D2" s="1">
-        <v>681.9170118713379</v>
+        <v>657.7212071228028</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -488,13 +488,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>2.14</v>
+        <v>-0.89</v>
       </c>
       <c r="C3" s="1">
-        <v>12.79</v>
+        <v>11.07</v>
       </c>
       <c r="D3" s="1">
-        <v>1261.177746458024</v>
+        <v>1242.076779157063</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -502,13 +502,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>2.15</v>
+        <v>-4.85</v>
       </c>
       <c r="C4" s="1">
-        <v>-38.4</v>
+        <v>-40.42</v>
       </c>
       <c r="D4" s="1">
-        <v>252.3617378620049</v>
+        <v>244.1154100140587</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -516,13 +516,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>-0.64</v>
+        <v>-3.15</v>
       </c>
       <c r="C5" s="1">
-        <v>-17.96</v>
+        <v>-19.37</v>
       </c>
       <c r="D5" s="1">
-        <v>210.7299412096491</v>
+        <v>207.1258462261812</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -530,13 +530,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>8.289999999999999</v>
+        <v>3.86</v>
       </c>
       <c r="C6" s="1">
-        <v>128.21</v>
+        <v>127.79</v>
       </c>
       <c r="D6" s="1">
-        <v>1286.713603658671</v>
+        <v>1284.492566079939</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -544,13 +544,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>-0.61</v>
+        <v>0.75</v>
       </c>
       <c r="C7" s="1">
-        <v>-31.42</v>
+        <v>-31.43</v>
       </c>
       <c r="D7" s="1">
-        <v>498.7693075478464</v>
+        <v>498.751945613536</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -558,13 +558,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="1">
-        <v>-1.81</v>
+        <v>-9.33</v>
       </c>
       <c r="C8" s="1">
-        <v>-30.93</v>
+        <v>-35.3</v>
       </c>
       <c r="D8" s="1">
-        <v>318.9457993599315</v>
+        <v>298.7874267198416</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -572,13 +572,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="1">
-        <v>-1.26</v>
+        <v>-3.06</v>
       </c>
       <c r="C9" s="1">
-        <v>-68.77</v>
+        <v>-69.33</v>
       </c>
       <c r="D9" s="1">
-        <v>376.9500045776367</v>
+        <v>370.2000045776367</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -586,13 +586,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="1">
-        <v>0.2</v>
+        <v>1.53</v>
       </c>
       <c r="C10" s="1">
-        <v>-2.83</v>
+        <v>-0.99</v>
       </c>
       <c r="D10" s="1">
-        <v>587.6999999999999</v>
+        <v>598.8</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -600,13 +600,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="1">
-        <v>1.85</v>
+        <v>-1</v>
       </c>
       <c r="C11" s="1">
-        <v>6.61</v>
+        <v>4.51</v>
       </c>
       <c r="D11" s="1">
-        <v>544.8237330000001</v>
+        <v>533.0465272023926</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -614,13 +614,13 @@
         <v>14</v>
       </c>
       <c r="B12" s="1">
-        <v>-5.65</v>
+        <v>-6.47</v>
       </c>
       <c r="C12" s="1">
-        <v>46.12</v>
+        <v>40.63</v>
       </c>
       <c r="D12" s="1">
-        <v>872.879927029953</v>
+        <v>838.4581796676636</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -628,13 +628,13 @@
         <v>15</v>
       </c>
       <c r="B13" s="1">
-        <v>7.78</v>
+        <v>3.94</v>
       </c>
       <c r="C13" s="1">
-        <v>-12.26</v>
+        <v>-13.49</v>
       </c>
       <c r="D13" s="1">
-        <v>1308.006625290777</v>
+        <v>1289.729481161152</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -642,13 +642,13 @@
         <v>16</v>
       </c>
       <c r="B14" s="1">
-        <v>-1.68</v>
+        <v>-6.03</v>
       </c>
       <c r="C14" s="1">
-        <v>37.09</v>
+        <v>30.87</v>
       </c>
       <c r="D14" s="1">
-        <v>240.6900110959508</v>
+        <v>229.7849179078067</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -656,13 +656,13 @@
         <v>17</v>
       </c>
       <c r="B15" s="1">
-        <v>-2.61</v>
+        <v>-4.25</v>
       </c>
       <c r="C15" s="1">
-        <v>-28.54</v>
+        <v>-29.91</v>
       </c>
       <c r="D15" s="1">
-        <v>497.9412672558684</v>
+        <v>488.4358902142849</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -670,13 +670,13 @@
         <v>18</v>
       </c>
       <c r="B16" s="1">
-        <v>-1.01</v>
+        <v>-2.53</v>
       </c>
       <c r="C16" s="1">
-        <v>26.58</v>
+        <v>23.03</v>
       </c>
       <c r="D16" s="1">
-        <v>567.4945843380776</v>
+        <v>550.5192316595765</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -684,13 +684,13 @@
         <v>19</v>
       </c>
       <c r="B17" s="1">
-        <v>-0.72</v>
+        <v>-8.1</v>
       </c>
       <c r="C17" s="1">
-        <v>-72.61</v>
+        <v>-73.67</v>
       </c>
       <c r="D17" s="1">
-        <v>104.856307376423</v>
+        <v>100.7946215176422</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -698,13 +698,13 @@
         <v>20</v>
       </c>
       <c r="B18" s="1">
-        <v>1.15</v>
+        <v>-1.52</v>
       </c>
       <c r="C18" s="1">
-        <v>-3.88</v>
+        <v>-5.67</v>
       </c>
       <c r="D18" s="1">
-        <v>9611.957607932152</v>
+        <v>9432.840034841578</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -715,10 +715,10 @@
         <v>22</v>
       </c>
       <c r="C19" s="1">
-        <v>1229.532809899639</v>
+        <v>1228.937934914572</v>
       </c>
       <c r="D19" s="1">
-        <v>1335.176621862619</v>
+        <v>1334.581746877552</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added back cash calcualtion since I'm a dumbo and removed it
</commit_message>
<xml_diff>
--- a/revamp/weekly_report.xlsx
+++ b/revamp/weekly_report.xlsx
@@ -474,13 +474,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>-5.15</v>
+        <v>-1.98</v>
       </c>
       <c r="C2" s="1">
-        <v>-36.08</v>
+        <v>-37.59</v>
       </c>
       <c r="D2" s="1">
-        <v>663.8674142456055</v>
+        <v>648.2265110778809</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -488,13 +488,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>1.62</v>
+        <v>-0.21</v>
       </c>
       <c r="C3" s="1">
-        <v>13.61</v>
+        <v>10.83</v>
       </c>
       <c r="D3" s="1">
-        <v>1265.177102904449</v>
+        <v>1234.248243933589</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -502,13 +502,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>-3.6</v>
+        <v>-2.09</v>
       </c>
       <c r="C4" s="1">
-        <v>-40.56</v>
+        <v>-41.67</v>
       </c>
       <c r="D4" s="1">
-        <v>242.5299666943591</v>
+        <v>238.0061077875848</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -516,13 +516,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>-1.24</v>
+        <v>-2.47</v>
       </c>
       <c r="C5" s="1">
-        <v>-18.82</v>
+        <v>-21.36</v>
       </c>
       <c r="D5" s="1">
-        <v>207.6741402090477</v>
+        <v>201.1710690622063</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -530,13 +530,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1">
-        <v>135.72</v>
+        <v>132.36</v>
       </c>
       <c r="D6" s="1">
-        <v>1323.610510147003</v>
+        <v>1304.761030125109</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -544,13 +544,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>4.04</v>
+        <v>3.5</v>
       </c>
       <c r="C7" s="1">
-        <v>-29.37</v>
+        <v>-29.03</v>
       </c>
       <c r="D7" s="1">
-        <v>511.621998071975</v>
+        <v>514.0410280970626</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -558,13 +558,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="1">
-        <v>-9.140000000000001</v>
+        <v>-0.1</v>
       </c>
       <c r="C8" s="1">
-        <v>-35.53</v>
+        <v>-35.37</v>
       </c>
       <c r="D8" s="1">
-        <v>296.478763208666</v>
+        <v>297.2563085738727</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -572,13 +572,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="1">
-        <v>-1.59</v>
+        <v>6.5</v>
       </c>
       <c r="C9" s="1">
-        <v>-69.25</v>
+        <v>-67.02</v>
       </c>
       <c r="D9" s="1">
-        <v>371.25</v>
+        <v>398.0999908447266</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -586,13 +586,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="1">
-        <v>-0.61</v>
+        <v>-4.08</v>
       </c>
       <c r="C10" s="1">
-        <v>-3.27</v>
+        <v>-5.51</v>
       </c>
       <c r="D10" s="1">
-        <v>585</v>
+        <v>571.5</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -600,13 +600,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="1">
-        <v>-4.55</v>
+        <v>0.08</v>
       </c>
       <c r="C11" s="1">
-        <v>1.76</v>
+        <v>2.04</v>
       </c>
       <c r="D11" s="1">
-        <v>520.1859742355347</v>
+        <v>521.6324033409119</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -614,13 +614,13 @@
         <v>14</v>
       </c>
       <c r="B12" s="1">
-        <v>-0.22</v>
+        <v>0.22</v>
       </c>
       <c r="C12" s="1">
-        <v>47.78</v>
+        <v>47.72</v>
       </c>
       <c r="D12" s="1">
-        <v>883.076379529953</v>
+        <v>882.6889677944183</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -628,13 +628,13 @@
         <v>15</v>
       </c>
       <c r="B13" s="1">
-        <v>8.449999999999999</v>
+        <v>7.79</v>
       </c>
       <c r="C13" s="1">
-        <v>-8.68</v>
+        <v>-6.75</v>
       </c>
       <c r="D13" s="1">
-        <v>1355.740950605465</v>
+        <v>1384.415729758644</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -642,13 +642,13 @@
         <v>16</v>
       </c>
       <c r="B14" s="1">
-        <v>-5.7</v>
+        <v>-2.16</v>
       </c>
       <c r="C14" s="1">
-        <v>28.6</v>
+        <v>28.04</v>
       </c>
       <c r="D14" s="1">
-        <v>224.8585821698778</v>
+        <v>895.50735367495</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -656,13 +656,13 @@
         <v>17</v>
       </c>
       <c r="B15" s="1">
-        <v>-0.42</v>
+        <v>0.64</v>
       </c>
       <c r="C15" s="1">
-        <v>-29.58</v>
+        <v>-29.46</v>
       </c>
       <c r="D15" s="1">
-        <v>488.6413656318956</v>
+        <v>489.5052869503047</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -670,13 +670,13 @@
         <v>18</v>
       </c>
       <c r="B16" s="1">
-        <v>-3.09</v>
+        <v>0.7</v>
       </c>
       <c r="C16" s="1">
-        <v>23.07</v>
+        <v>24.42</v>
       </c>
       <c r="D16" s="1">
-        <v>551.9378144393921</v>
+        <v>557.9988966590881</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -684,13 +684,13 @@
         <v>19</v>
       </c>
       <c r="B17" s="1">
-        <v>-2.98</v>
+        <v>-2.08</v>
       </c>
       <c r="C17" s="1">
-        <v>-72.87</v>
+        <v>-74.22</v>
       </c>
       <c r="D17" s="1">
-        <v>103.436519223307</v>
+        <v>98.28432993479093</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -698,13 +698,13 @@
         <v>20</v>
       </c>
       <c r="B18" s="1">
-        <v>0.6</v>
+        <v>1.11</v>
       </c>
       <c r="C18" s="1">
-        <v>-4.05</v>
+        <v>2.37</v>
       </c>
       <c r="D18" s="1">
-        <v>9595.087481316532</v>
+        <v>10237.34325761514</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -715,10 +715,10 @@
         <v>22</v>
       </c>
       <c r="C19" s="1">
-        <v>1232.549681855884</v>
+        <v>1323.367396896345</v>
       </c>
       <c r="D19" s="1">
-        <v>1338.193493818864</v>
+        <v>912.6268620576598</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed dividend cash position
</commit_message>
<xml_diff>
--- a/revamp/weekly_report.xlsx
+++ b/revamp/weekly_report.xlsx
@@ -474,13 +474,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>-1.98</v>
+        <v>-0.1</v>
       </c>
       <c r="C2" s="1">
-        <v>-37.59</v>
+        <v>-35.56</v>
       </c>
       <c r="D2" s="1">
-        <v>648.2265110778809</v>
+        <v>669.3133905029297</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -488,13 +488,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>-0.21</v>
+        <v>-1.37</v>
       </c>
       <c r="C3" s="1">
-        <v>10.83</v>
+        <v>10.27</v>
       </c>
       <c r="D3" s="1">
-        <v>1234.248243933589</v>
+        <v>1227.933637446762</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -502,13 +502,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>-2.09</v>
+        <v>0.73</v>
       </c>
       <c r="C4" s="1">
-        <v>-41.67</v>
+        <v>-40.41</v>
       </c>
       <c r="D4" s="1">
-        <v>238.0061077875848</v>
+        <v>243.1582970761009</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -516,13 +516,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>-2.47</v>
+        <v>-3.59</v>
       </c>
       <c r="C5" s="1">
-        <v>-21.36</v>
+        <v>-22.77</v>
       </c>
       <c r="D5" s="1">
-        <v>201.1710690622063</v>
+        <v>197.5661178723541</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -530,13 +530,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>3.96</v>
       </c>
       <c r="C6" s="1">
-        <v>132.36</v>
+        <v>141.47</v>
       </c>
       <c r="D6" s="1">
-        <v>1304.761030125109</v>
+        <v>1355.89027344652</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -544,13 +544,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>3.5</v>
+        <v>3.38</v>
       </c>
       <c r="C7" s="1">
-        <v>-29.03</v>
+        <v>-26.42</v>
       </c>
       <c r="D7" s="1">
-        <v>514.0410280970626</v>
+        <v>532.9533531413073</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -558,13 +558,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="1">
-        <v>-0.1</v>
+        <v>4.71</v>
       </c>
       <c r="C8" s="1">
-        <v>-35.37</v>
+        <v>-31.26</v>
       </c>
       <c r="D8" s="1">
-        <v>297.2563085738727</v>
+        <v>316.1528864099996</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -572,13 +572,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="1">
-        <v>6.5</v>
+        <v>9.050000000000001</v>
       </c>
       <c r="C9" s="1">
-        <v>-67.02</v>
+        <v>-65.56999999999999</v>
       </c>
       <c r="D9" s="1">
-        <v>398.0999908447266</v>
+        <v>415.6500091552734</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -586,13 +586,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="1">
-        <v>-4.08</v>
+        <v>3.49</v>
       </c>
       <c r="C10" s="1">
-        <v>-5.51</v>
+        <v>-1.44</v>
       </c>
       <c r="D10" s="1">
-        <v>571.5</v>
+        <v>596.1</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -600,13 +600,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="1">
-        <v>0.08</v>
+        <v>-3.48</v>
       </c>
       <c r="C11" s="1">
-        <v>2.04</v>
+        <v>1.01</v>
       </c>
       <c r="D11" s="1">
-        <v>521.6324033409119</v>
+        <v>516.3633672706604</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -614,13 +614,13 @@
         <v>14</v>
       </c>
       <c r="B12" s="1">
-        <v>0.22</v>
+        <v>-1.72</v>
       </c>
       <c r="C12" s="1">
-        <v>47.72</v>
+        <v>47.91</v>
       </c>
       <c r="D12" s="1">
-        <v>882.6889677944183</v>
+        <v>883.8513015289307</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -628,13 +628,13 @@
         <v>15</v>
       </c>
       <c r="B13" s="1">
-        <v>7.79</v>
+        <v>-1.4</v>
       </c>
       <c r="C13" s="1">
-        <v>-6.75</v>
+        <v>-8.199999999999999</v>
       </c>
       <c r="D13" s="1">
-        <v>1384.415729758644</v>
+        <v>1362.895983432379</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -642,13 +642,13 @@
         <v>16</v>
       </c>
       <c r="B14" s="1">
-        <v>-2.16</v>
+        <v>3.31</v>
       </c>
       <c r="C14" s="1">
-        <v>28.04</v>
+        <v>33.14</v>
       </c>
       <c r="D14" s="1">
-        <v>895.50735367495</v>
+        <v>931.1642939068718</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -656,13 +656,13 @@
         <v>17</v>
       </c>
       <c r="B15" s="1">
-        <v>0.64</v>
+        <v>-4.96</v>
       </c>
       <c r="C15" s="1">
-        <v>-29.46</v>
+        <v>-32.72</v>
       </c>
       <c r="D15" s="1">
-        <v>489.5052869503047</v>
+        <v>466.8702122518299</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -670,13 +670,13 @@
         <v>18</v>
       </c>
       <c r="B16" s="1">
-        <v>0.7</v>
+        <v>3.97</v>
       </c>
       <c r="C16" s="1">
-        <v>24.42</v>
+        <v>27.61</v>
       </c>
       <c r="D16" s="1">
-        <v>557.9988966590881</v>
+        <v>572.299296390152</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -684,13 +684,13 @@
         <v>19</v>
       </c>
       <c r="B17" s="1">
-        <v>-2.08</v>
+        <v>3.05</v>
       </c>
       <c r="C17" s="1">
-        <v>-74.22</v>
+        <v>-71.89</v>
       </c>
       <c r="D17" s="1">
-        <v>98.28432993479093</v>
+        <v>107.1592958419346</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -698,13 +698,13 @@
         <v>20</v>
       </c>
       <c r="B18" s="1">
-        <v>1.11</v>
+        <v>0.83</v>
       </c>
       <c r="C18" s="1">
-        <v>2.37</v>
+        <v>3.95</v>
       </c>
       <c r="D18" s="1">
-        <v>10237.34325761514</v>
+        <v>10395.321715674</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -715,10 +715,10 @@
         <v>22</v>
       </c>
       <c r="C19" s="1">
-        <v>1323.367396896345</v>
+        <v>1333.465581704775</v>
       </c>
       <c r="D19" s="1">
-        <v>912.6268620576598</v>
+        <v>922.7250468660891</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
portfolio dump has an extra summary sheet now
</commit_message>
<xml_diff>
--- a/revamp/weekly_report.xlsx
+++ b/revamp/weekly_report.xlsx
@@ -474,13 +474,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>-0.1</v>
+        <v>0.51</v>
       </c>
       <c r="C2" s="1">
-        <v>-35.56</v>
+        <v>-36.61</v>
       </c>
       <c r="D2" s="1">
-        <v>669.3133905029297</v>
+        <v>658.4213786315918</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -488,13 +488,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>-1.37</v>
+        <v>0.09</v>
       </c>
       <c r="C3" s="1">
-        <v>10.27</v>
+        <v>11.15</v>
       </c>
       <c r="D3" s="1">
-        <v>1227.933637446762</v>
+        <v>1237.782521437694</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -502,13 +502,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>0.73</v>
+        <v>0.49</v>
       </c>
       <c r="C4" s="1">
-        <v>-40.41</v>
+        <v>-39.98</v>
       </c>
       <c r="D4" s="1">
-        <v>243.1582970761009</v>
+        <v>244.9175742082712</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -516,13 +516,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>-3.59</v>
+        <v>-0.39</v>
       </c>
       <c r="C5" s="1">
-        <v>-22.77</v>
+        <v>-22.16</v>
       </c>
       <c r="D5" s="1">
-        <v>197.5661178723541</v>
+        <v>199.1211951205687</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -530,13 +530,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>3.96</v>
+        <v>2.04</v>
       </c>
       <c r="C6" s="1">
-        <v>141.47</v>
+        <v>139.73</v>
       </c>
       <c r="D6" s="1">
-        <v>1355.89027344652</v>
+        <v>1346.135633020761</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -544,13 +544,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>3.38</v>
+        <v>1.86</v>
       </c>
       <c r="C7" s="1">
-        <v>-26.42</v>
+        <v>-26.28</v>
       </c>
       <c r="D7" s="1">
-        <v>532.9533531413073</v>
+        <v>533.99789997018</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -558,13 +558,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="1">
-        <v>4.71</v>
+        <v>2.54</v>
       </c>
       <c r="C8" s="1">
-        <v>-31.26</v>
+        <v>-31.29</v>
       </c>
       <c r="D8" s="1">
-        <v>316.1528864099996</v>
+        <v>316.0115210622402</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -572,13 +572,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="1">
-        <v>9.050000000000001</v>
+        <v>8.77</v>
       </c>
       <c r="C9" s="1">
-        <v>-65.56999999999999</v>
+        <v>-64.26000000000001</v>
       </c>
       <c r="D9" s="1">
-        <v>415.6500091552734</v>
+        <v>431.4000091552734</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -586,13 +586,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="1">
-        <v>3.49</v>
+        <v>-0.7</v>
       </c>
       <c r="C10" s="1">
-        <v>-1.44</v>
+        <v>-2.13</v>
       </c>
       <c r="D10" s="1">
-        <v>596.1</v>
+        <v>591.9</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -600,13 +600,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="1">
-        <v>-3.48</v>
+        <v>0.8</v>
       </c>
       <c r="C11" s="1">
-        <v>1.01</v>
+        <v>1.96</v>
       </c>
       <c r="D11" s="1">
-        <v>516.3633672706604</v>
+        <v>521.2191378822326</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -614,13 +614,13 @@
         <v>14</v>
       </c>
       <c r="B12" s="1">
-        <v>-1.72</v>
+        <v>-2.15</v>
       </c>
       <c r="C12" s="1">
-        <v>47.91</v>
+        <v>45.26</v>
       </c>
       <c r="D12" s="1">
-        <v>883.8513015289307</v>
+        <v>867.966730676651</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -628,13 +628,13 @@
         <v>15</v>
       </c>
       <c r="B13" s="1">
-        <v>-1.4</v>
+        <v>-1.28</v>
       </c>
       <c r="C13" s="1">
-        <v>-8.199999999999999</v>
+        <v>-6.21</v>
       </c>
       <c r="D13" s="1">
-        <v>1362.895983432379</v>
+        <v>1392.426816291997</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -642,13 +642,13 @@
         <v>16</v>
       </c>
       <c r="B14" s="1">
-        <v>3.31</v>
+        <v>-0.5600000000000001</v>
       </c>
       <c r="C14" s="1">
-        <v>33.14</v>
+        <v>30.6</v>
       </c>
       <c r="D14" s="1">
-        <v>931.1642939068718</v>
+        <v>913.414410029291</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -656,13 +656,13 @@
         <v>17</v>
       </c>
       <c r="B15" s="1">
-        <v>-4.96</v>
+        <v>-1.97</v>
       </c>
       <c r="C15" s="1">
-        <v>-32.72</v>
+        <v>-32.95</v>
       </c>
       <c r="D15" s="1">
-        <v>466.8702122518299</v>
+        <v>465.3151275135048</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -670,13 +670,13 @@
         <v>18</v>
       </c>
       <c r="B16" s="1">
-        <v>3.97</v>
+        <v>0.3</v>
       </c>
       <c r="C16" s="1">
-        <v>27.61</v>
+        <v>26.28</v>
       </c>
       <c r="D16" s="1">
-        <v>572.299296390152</v>
+        <v>566.33290277462</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -684,13 +684,13 @@
         <v>19</v>
       </c>
       <c r="B17" s="1">
-        <v>3.05</v>
+        <v>4.48</v>
       </c>
       <c r="C17" s="1">
-        <v>-71.89</v>
+        <v>-72.03</v>
       </c>
       <c r="D17" s="1">
-        <v>107.1592958419346</v>
+        <v>106.6252210095424</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -698,13 +698,13 @@
         <v>20</v>
       </c>
       <c r="B18" s="1">
-        <v>0.83</v>
+        <v>0.33</v>
       </c>
       <c r="C18" s="1">
-        <v>3.95</v>
+        <v>3.93</v>
       </c>
       <c r="D18" s="1">
-        <v>10395.321715674</v>
+        <v>10392.98807878442</v>
       </c>
     </row>
     <row r="19" spans="1:4">

</xml_diff>

<commit_message>
making sure it works
</commit_message>
<xml_diff>
--- a/revamp/weekly_report.xlsx
+++ b/revamp/weekly_report.xlsx
@@ -474,13 +474,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>-2.22</v>
+        <v>0.52</v>
       </c>
       <c r="C2" s="1">
-        <v>6098.5</v>
+        <v>-22.46</v>
       </c>
       <c r="D2" s="1">
-        <v>643.7950000000001</v>
+        <v>805.3855738830566</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -488,13 +488,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>1.05</v>
+        <v>-0.99</v>
       </c>
       <c r="C3" s="1">
-        <v>11.89</v>
+        <v>17.6</v>
       </c>
       <c r="D3" s="1">
-        <v>1245.950648621864</v>
+        <v>1325.573728547231</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -502,13 +502,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>3.24</v>
+        <v>1.74</v>
       </c>
       <c r="C4" s="1">
-        <v>-37.7</v>
+        <v>-34.19</v>
       </c>
       <c r="D4" s="1">
-        <v>254.2166481428698</v>
+        <v>271.8245054743797</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -516,13 +516,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>-1.76</v>
+        <v>-1.23</v>
       </c>
       <c r="C5" s="1">
-        <v>-22.66</v>
+        <v>-31.14</v>
       </c>
       <c r="D5" s="1">
-        <v>197.8488530619391</v>
+        <v>178.3013508430562</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -530,13 +530,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>2.87</v>
+        <v>-2.34</v>
       </c>
       <c r="C6" s="1">
-        <v>145.01</v>
+        <v>152.75</v>
       </c>
       <c r="D6" s="1">
-        <v>1375.776480622023</v>
+        <v>1436.618495895817</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -544,13 +544,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>13.89</v>
+        <v>4.85</v>
       </c>
       <c r="C7" s="1">
-        <v>-16.1</v>
+        <v>-7.13</v>
       </c>
       <c r="D7" s="1">
-        <v>607.722948839229</v>
+        <v>680.9286308111443</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -558,13 +558,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="1">
-        <v>4.51</v>
+        <v>5.4</v>
       </c>
       <c r="C8" s="1">
-        <v>-27.88</v>
+        <v>-21.03</v>
       </c>
       <c r="D8" s="1">
-        <v>331.6801729019574</v>
+        <v>367.6451586415828</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -572,13 +572,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="1">
-        <v>-3.72</v>
+        <v>3.67</v>
       </c>
       <c r="C9" s="1">
-        <v>3340.82</v>
+        <v>-64.54000000000001</v>
       </c>
       <c r="D9" s="1">
-        <v>415.3499908447266</v>
+        <v>428.0999908447266</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -586,13 +586,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="1">
-        <v>-0.41</v>
+        <v>-2.33</v>
       </c>
       <c r="C10" s="1">
-        <v>9647.02</v>
+        <v>-0.4</v>
       </c>
       <c r="D10" s="1">
-        <v>589.5</v>
+        <v>602.4</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -600,13 +600,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="1">
-        <v>1.19</v>
+        <v>-0.15</v>
       </c>
       <c r="C11" s="1">
-        <v>3.17</v>
+        <v>4.85</v>
       </c>
       <c r="D11" s="1">
-        <v>527.4179621177673</v>
+        <v>532.9424989723205</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -614,13 +614,13 @@
         <v>14</v>
       </c>
       <c r="B12" s="1">
-        <v>0.28</v>
+        <v>-1.18</v>
       </c>
       <c r="C12" s="1">
-        <v>45.67</v>
+        <v>36.22</v>
       </c>
       <c r="D12" s="1">
-        <v>870.4204697055817</v>
+        <v>809.3524568252564</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -628,13 +628,13 @@
         <v>15</v>
       </c>
       <c r="B13" s="1">
-        <v>-0.88</v>
+        <v>-2.81</v>
       </c>
       <c r="C13" s="1">
-        <v>-8.33</v>
+        <v>-20.01</v>
       </c>
       <c r="D13" s="1">
-        <v>1360.955984916332</v>
+        <v>1201.99974420556</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -642,13 +642,13 @@
         <v>16</v>
       </c>
       <c r="B14" s="1">
-        <v>-5.79</v>
+        <v>4.16</v>
       </c>
       <c r="C14" s="1">
-        <v>26.42</v>
+        <v>43.54</v>
       </c>
       <c r="D14" s="1">
-        <v>884.1977064080143</v>
+        <v>1016.161875359902</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -656,13 +656,13 @@
         <v>17</v>
       </c>
       <c r="B15" s="1">
-        <v>1.03</v>
+        <v>0.33</v>
       </c>
       <c r="C15" s="1">
-        <v>-31.35</v>
+        <v>-30.9</v>
       </c>
       <c r="D15" s="1">
-        <v>476.3734785802737</v>
+        <v>485.3440982540862</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -670,13 +670,13 @@
         <v>18</v>
       </c>
       <c r="B16" s="1">
-        <v>-0.52</v>
+        <v>0.87</v>
       </c>
       <c r="C16" s="1">
-        <v>25.63</v>
+        <v>34.03</v>
       </c>
       <c r="D16" s="1">
-        <v>563.3970863958359</v>
+        <v>597.668439994812</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -684,13 +684,13 @@
         <v>19</v>
       </c>
       <c r="B17" s="1">
-        <v>3.24</v>
+        <v>0.63</v>
       </c>
       <c r="C17" s="1">
-        <v>-71.64</v>
+        <v>-65.15000000000001</v>
       </c>
       <c r="D17" s="1">
-        <v>108.1174787017817</v>
+        <v>134.4812603407771</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -698,13 +698,13 @@
         <v>20</v>
       </c>
       <c r="B18" s="1">
-        <v>0.66</v>
+        <v>0.12</v>
       </c>
       <c r="C18" s="1">
-        <v>4.53</v>
+        <v>8.75</v>
       </c>
       <c r="D18" s="1">
-        <v>10452.7209098602</v>
+        <v>10874.72780889371</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -715,10 +715,10 @@
         <v>22</v>
       </c>
       <c r="C19" s="1">
-        <v>1333.465581704775</v>
+        <v>1346.635221111907</v>
       </c>
       <c r="D19" s="1">
-        <v>3744.774496901183</v>
+        <v>935.8946862732214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>